<commit_message>
F Roosevelt 2 edits
</commit_message>
<xml_diff>
--- a/Team-Roles.xlsx
+++ b/Team-Roles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cde73a511afdd567/Documents/GitHub/Pres-Inaug-Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taishanahan/Desktop/Pres-Inaug-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{44B49F87-A270-2946-8C69-48FC9B24FD1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51C56849-C904-4785-8C03-59081DDEBEC7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816E4DC0-A5D3-7547-8F13-C44F0FDD4C21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7EE72846-32B2-FA4F-942E-A4AC999FAD54}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="15500" xr2:uid="{7EE72846-32B2-FA4F-942E-A4AC999FAD54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -527,19 +527,19 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.69921875" customWidth="1"/>
-    <col min="2" max="2" width="8.69921875" customWidth="1"/>
-    <col min="3" max="3" width="17.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.296875" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>28</v>
       </c>
@@ -559,7 +559,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -579,7 +579,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -599,7 +599,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -619,7 +619,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -639,7 +639,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -659,7 +659,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -679,7 +679,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -699,7 +699,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -719,7 +719,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -739,7 +739,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -759,7 +759,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -779,7 +779,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -796,10 +796,10 @@
         <v>7</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -819,7 +819,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -839,7 +839,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -859,7 +859,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -879,7 +879,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -899,7 +899,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -919,7 +919,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -939,7 +939,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -959,7 +959,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -979,7 +979,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -999,7 +999,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1159,7 +1159,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1179,7 +1179,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1219,7 +1219,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>

</xml_diff>